<commit_message>
change data annotation template
</commit_message>
<xml_diff>
--- a/src/main/resources/websheet/datacommentdemo.xlsx
+++ b/src/main/resources/websheet/datacommentdemo.xlsx
@@ -44,7 +44,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>tie:each(items="departments", var="department", length="8" allowAdd="false")</t>
+          <t>tie:each(items="departments", var="department", length="8" allowAdd="true")</t>
         </r>
       </text>
     </comment>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Department:</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>${department.chief.name}</t>
-  </si>
-  <si>
-    <t>${department.headcount}</t>
   </si>
   <si>
     <t>${employee.name}</t>
@@ -1099,7 +1096,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1137,8 +1134,9 @@
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>11</v>
+      <c r="B4" s="21">
+        <f>COUNT((E8))</f>
+        <v>0</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="22"/>
@@ -1149,7 +1147,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="24"/>
@@ -1181,16 +1179,16 @@
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="C8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="D8" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>15</v>
       </c>
       <c r="E8" s="13" t="e">
         <f>C8*(1+D8)</f>
@@ -1199,7 +1197,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11">

</xml_diff>

<commit_message>
migrate to poi 3.15
</commit_message>
<xml_diff>
--- a/src/main/resources/websheet/datacommentdemo.xlsx
+++ b/src/main/resources/websheet/datacommentdemo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="10710" tabRatio="548"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="10710" tabRatio="548"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -58,6 +58,19 @@
             <charset val="1"/>
           </rPr>
           <t>Department name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$save{department.headAccount}</t>
         </r>
       </text>
     </comment>
@@ -178,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_)@"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -381,6 +394,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="18">
@@ -1096,7 +1115,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Initial the 1.0.0 which has a huge imporvement on data binding part.
</commit_message>
<xml_diff>
--- a/src/main/resources/websheet/datacommentdemo.xlsx
+++ b/src/main/resources/websheet/datacommentdemo.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="10716" tabRatio="548"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20736" windowHeight="10656" tabRatio="548"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="My_Print_Area" localSheetId="0">Template!$A$1:$F$10</definedName>
+    <definedName name="My_Print_Area" localSheetId="0">Template!$A$1:$H$10</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -87,7 +87,61 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0">
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$widget.calendar{showOn="button" pattern="yyyy/MM/dd" readonlyInput="true"}</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$widget.dropdown{itemLabels="Male;Female" itemValues="M;F" }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$widget.inputnumber{symbol=" years" symbolPosition="s" minValue="0" maxValue="999" decimalPlaces="2"}</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>$init{employee.initbonus}</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="G9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Department:</t>
   </si>
@@ -148,9 +202,6 @@
     <t>Employee</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>Payment</t>
   </si>
   <si>
@@ -169,9 +220,6 @@
     <t>${employee.name}</t>
   </si>
   <si>
-    <t>${employee.age} years</t>
-  </si>
-  <si>
     <t>${employee.payment}</t>
   </si>
   <si>
@@ -181,7 +229,25 @@
     <t>SUB TOTALS</t>
   </si>
   <si>
-    <t>$init{employee.initbonus} ${employee.bonus}</t>
+    <t>${employee.birthDate}</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>${employee.bonus}</t>
+  </si>
+  <si>
+    <t>Working Time</t>
+  </si>
+  <si>
+    <t>${employee.worktime}</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>${employee.sex}</t>
   </si>
 </sst>
 </file>
@@ -191,7 +257,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_)@"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -204,23 +270,6 @@
       <color indexed="54"/>
       <name val="Cambria"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color indexed="54"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -396,6 +445,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -659,118 +722,117 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="10" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="10" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="11" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="11" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1115,138 +1177,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.36328125" customWidth="1"/>
     <col min="2" max="2" width="14.36328125" customWidth="1"/>
-    <col min="3" max="4" width="11.36328125" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" customWidth="1"/>
+    <col min="5" max="6" width="11.36328125" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="2"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
-    <row r="3" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="20" t="s">
+    <row r="4" spans="1:7" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21">
+        <f>COUNT((G8))</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" ht="37.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="2"/>
+      <c r="B8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="12" t="e">
+        <f>E8*(1+F8)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="22">
-        <f>COUNT((E8))</f>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10">
+        <f>SUM((E8))</f>
         <v>0</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="2"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="11" t="e">
+        <f>SUM((G8))</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="8" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="13" t="e">
-        <f>C8*(1+D8)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11">
-        <f>SUM((C8))</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="12" t="e">
-        <f>SUM((E8))</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="16" t="e">
-        <f>SUM((E9))</f>
+      <c r="G10" s="14" t="e">
+        <f>SUM((G9))</f>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <pageMargins left="0.69861111111111107" right="0.69861111111111107" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>